<commit_message>
Add sample question sub-type
</commit_message>
<xml_diff>
--- a/SC 1 - 10 - Commented.xlsx
+++ b/SC 1 - 10 - Commented.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="111">
   <si>
     <t>Stimulus</t>
   </si>
@@ -72,213 +72,7 @@
     <t>E. Cụm "each had been" không đúng về dùng thì quá khứ hoàn thành.</t>
   </si>
   <si>
-    <t>A.      was the only one of the five-nation Iroquois League who sided</t>
-  </si>
-  <si>
-    <t>B.      was alone of the five-nation Iroquois League when they sided</t>
-  </si>
-  <si>
-    <t>C.      alone among the five-nation Iroquois League sided</t>
-  </si>
-  <si>
-    <t>D.     were the only ones out of the five nations of Iroquois League in siding</t>
-  </si>
-  <si>
-    <t>E.      only of the five-nation Iroquois League had sided</t>
-  </si>
-  <si>
-    <t>A. Who chỉ modify cho người, không thể modify cho tổ chức Iroquois League.</t>
-  </si>
-  <si>
-    <t>D. Chủ ngữ của câu là "the Oneida", vì thế vị ngữ không thể chia số nhiều "were"</t>
-  </si>
-  <si>
-    <t>B. "They" là pronoun chỉ tới five-nation Iroquois League, nhưng không hợp lý về nghĩa: Oneida là bên duy nhất đứng về phía các thuộc địa trong Cách mạng Mỹ, không phải là Iroquois League.</t>
-  </si>
-  <si>
-    <t>C. Đáp án đúng.</t>
-  </si>
-  <si>
-    <t>E. Dùng thì quá khứ hoàn thành với "had sided" là không hợp lý, vì đây là một sự kiện diễn ra sau sự kiện "influenced by the Protested missionary Samuel Kirkland".</t>
-  </si>
-  <si>
-    <t>C. Đáp án đúng. "Alone among the five-nation Iroquois League" là modifier của Oneida, "sided" là vị ngữ của câu.</t>
-  </si>
-  <si>
-    <t>A. their horny jaws function for teeth</t>
-  </si>
-  <si>
-    <t>B. its horny jaws function for teeth</t>
-  </si>
-  <si>
-    <t>C. its horny jaws function as do teeth</t>
-  </si>
-  <si>
-    <t>D the horny jaws function as teeth do</t>
-  </si>
-  <si>
-    <r>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>the horny jaws function as teeth</t>
-    </r>
-  </si>
-  <si>
-    <t>A. Function for teeth là không đúng, phải là  Function as teeth (có chức năng như răng).</t>
-  </si>
-  <si>
-    <t>B. Danh từ của pronoun là "turtle species" (số nhiều), vì thế pronoun không thể là its.</t>
-  </si>
-  <si>
-    <t>C. Danh từ của pronoun là "turtle species" (số nhiều), vì thế pronoun không thể là its.</t>
-  </si>
-  <si>
-    <t>D. So sánh "horny jaws" với "teeth" (so sánh 2 danh từ), vì thế thêm "do" vào sau teeth là sai</t>
-  </si>
-  <si>
-    <t>E. Đáp án đúng.</t>
-  </si>
-  <si>
-    <t>A. the Aramaic script with it, from which was derived both northern and</t>
-  </si>
-  <si>
-    <t>B. the Aramaic script with it, and from which deriving both the northern and the</t>
-  </si>
-  <si>
-    <t>C. with it the Aramaic script, from which derive both the northern and the</t>
-  </si>
-  <si>
-    <t>D. with it the Aramaic script, from which derives both northern and</t>
-  </si>
-  <si>
-    <t>E. with it the Aramaic script, and deriving from it both the northern and</t>
-  </si>
-  <si>
-    <t>A. "from which" phải modify cho danh từ kề với nó, mà theo nghĩa của câu thì bảng chữ cái ở nam và bắc Ấn Độ đều xuất phát từ Aramaic script, vì thế đặt "it" ở trước "from which" là sai</t>
-  </si>
-  <si>
-    <t>D. "Derives" là động từ của cụm "both northern and southern India alphabets" - một danh từ số nhiều, vì thế "derive" phải chia số ít.</t>
-  </si>
-  <si>
-    <t>B. "and" là dấu hiệu của Parallellism, nhưng cụm "bringing" và cụm "from which deriving" không song song về mặt nghĩa với nhau.</t>
-  </si>
-  <si>
-    <t>E. "and" là dấu hiệu của Parallellism, nhưng cụm "bringing" và cụm "deriving" không song song về mặt nghĩa với nhau.</t>
-  </si>
-  <si>
-    <r>
-      <t>A.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>　</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>annually by preventing illness among employees and gain as much as $200 billion through improving performance of workers if they simply provided</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>　</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>annually if they prevented employee illness and gain as much as $200 billion through worker performance improved by simply providing</t>
-    </r>
-  </si>
-  <si>
-    <t>C.  annually in employee illness prevention and gain as much as $200 billion through worker performance improved by simply providing</t>
-  </si>
-  <si>
-    <t>D. in employee illness prevention and gain as much as $200 billion through improving performance of workers if they simply provided</t>
-  </si>
-  <si>
-    <t>E. by preventing illness among employees and gain as much as $200 billion through improved worker performance if they simply provided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. Vì đã có "each year" nên "annually" là redundant </t>
-  </si>
-  <si>
-    <t>B. "annually" là redundant. Đây là câu điều kiện loại II nên phải dùng mệnh đề if + V-ed</t>
-  </si>
-  <si>
-    <t>C. "annually" là redundant. Đây là câu điều kiện loại II nên phải dùng mệnh đề if + V-ed</t>
-  </si>
-  <si>
-    <t>D. "save as much as $58 billion in employee illness prevention", tức "tiết kiện 58 tỷ đôla trong phòng chống bệnh tật cho công nhân" là không hợp lý về nghĩa trong câu này</t>
-  </si>
-  <si>
-    <t>Wordy không tính là lỗi, nhưng Redundancy tính là lỗi.</t>
-  </si>
-  <si>
-    <t>A  Women are expected to be the majority of student entering law school this fall, a trend ultimately placing</t>
-  </si>
-  <si>
-    <t>B  The majority of students entering law school this fall are expected to be women, a trend that will ultimately place</t>
-  </si>
-  <si>
-    <t>C  The majority of students entering law school this fall are expected to be women, which will ultimately place</t>
-  </si>
-  <si>
-    <t>D  It is expected that the majority of students entering law school this fall will be women, a trend ultimately placing</t>
-  </si>
-  <si>
-    <t>E  It is expected for the women to be the majority of students entering law school this fall, which will ultimately place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. "A trend ultimately placing" là một cụm danh từ, không phải một cụm chủ - vị. Nhưng nghĩa của câu tập trung vào ý xu hướng này (phụ nữ chiếm phần lớn học sinh trường luật) sẽ đặt nhiều phụ nữ trong vị trí lãnh đạo trong chính trị và kinh doanh, vì thế cần có một cụm chủ - vị ở cụm "a trend ..." </t>
-  </si>
-  <si>
     <t>B. Đáp án đúng.</t>
-  </si>
-  <si>
-    <t>C. "which" chỉ modify cho vật ở ngay cạnh nó, không thể modify cho "women"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. "A trend ultimately placing" là một cụm danh từ, không phải một cụm chủ - vị. Nhưng nghĩa của câu tập trung vào ý xu hướng này (phụ nữ chiếm phần lớn học sinh trường luật) sẽ đặt nhiều phụ nữ trong vị trí lãnh đạo trong chính trị và kinh doanh, vì thế cần có một cụm chủ - vị ở cụm "a trend ..." </t>
-  </si>
-  <si>
-    <t>E. "which" trong câu này modify cho "this fall", nhưng sẽ không hợp lý về mặt nghĩa: mùa thu cuối cùng sẽ đặt nhiều phụ nữ trong vị trí lãnh đạo.</t>
   </si>
   <si>
     <r>
@@ -537,133 +331,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Greatly influenced by the Protested missionary Samuel Kirkland, the Oneida </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>was the only one of the five-nation Iroquois League who sided</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with the colonists during the American Revolution. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Although the turtle has been toothless for more than 150 million years, in some contemporary turtle species the moderately sharp and jagged edges of </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>their horny jaws function for teeth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The Achaemenid empire of Persia reached the Indus Valley in the fifth century B.C., bringing the </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aramaic script with it, from which was derived both northern</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and southern India alphabets.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Each year companies in the United State could save as much as $58 billion </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">annually by preventing illness among employees and gain as much as $200 billion through improving performance of workers if they simply provided </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>offices with cleaner air.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Women are expected to be the majority of student entering law school this fall, a trend ultimately placing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>more women in leadership position in politics and business.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">The yield per acre of coffee berries varies </t>
     </r>
     <r>
@@ -766,25 +433,154 @@
       <t xml:space="preserve"> learn new songs.</t>
     </r>
   </si>
+  <si>
+    <t>If an object travels at five feet per second, how many feet does it travel in one hour?</t>
+  </si>
+  <si>
+    <t>A.. 30</t>
+  </si>
+  <si>
+    <t>B. 300</t>
+  </si>
+  <si>
+    <t>C. 720</t>
+  </si>
+  <si>
+    <t>D. 1800</t>
+  </si>
+  <si>
+    <t>E. 18000</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>A. Đáp án sai</t>
+  </si>
+  <si>
+    <t>B. Đáp án sai</t>
+  </si>
+  <si>
+    <t>C. Đáp án sai</t>
+  </si>
+  <si>
+    <t>D. Đáp án sai</t>
+  </si>
+  <si>
+    <t>E. Đáp án đúng</t>
+  </si>
+  <si>
+    <t>Should we really care for the greatest actors of the past could we have them before us? Should we find them too different from our accent of thought, of feeling, of speech, in a thousand minute particulars which are of the essence of all three? Dr. Doran's long and interesting records of the triumphs of Garrick, and other less familiar, but in their day hardly less astonishing, players, do not relieve one of the doubt. Garrick himself, as sometimes happens with people who have been the subject of much anecdote and other conversation, here as elsewhere, bears no very distinct figure. One hardly sees the wood for the trees. On the other hand, the account of Betterton, "perhaps the greatest of English actors," is delightfully fresh. That intimate friend of Dryden, Tillatson, Pope, who executed a copy of the actor's portrait by Kneller which is still extant, was worthy of their friendship; his career brings out the best elements in stage life. The stage in these volumes presents itself indeed not merely as a mirror of life, but as an illustration of the utmost intensity of life, in the fortunes and characters of the players. Ups and downs, generosity, dark fates, the most delicate goodness, have nowhere been more prominent than in the private existence of those devoted to the public mimicry of men and women. Contact with the stage, almost throughout its history, presents itself as a kind of touchstone, to bring out the bizarrerie, the theatrical tricks and contrasts, of the actual world.
+Adapted from an essay by W H Pater</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In the expression “One hardly sees the wood for the trees”, the author apparently intends the word trees to be analogous to</t>
+  </si>
+  <si>
+    <t>B. Đáp án đúng</t>
+  </si>
+  <si>
+    <t>E. Đáp án sai</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>The doubt referred to in line 7 concerns whether</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Information supplied in the passage is sufficient to answer which of the following questions?
+I Who did Doran think was probably the best English actor?
+II What did Doran think of Garrick?
+III Would the author give a definite answer to the first question posed in the passage?</t>
+  </si>
+  <si>
+    <t>What is the average (arithmetic mean) of all the multiples of ten from 10 to 190 inclusive?</t>
+  </si>
+  <si>
+    <t>C. Đáp án đúng</t>
+  </si>
+  <si>
+    <t>A. Đáp án đúng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.  features of Doran’s language style </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. details learned from oral sources </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C. personality of a famous actor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D. detail’s of Garrick’s life </t>
+  </si>
+  <si>
+    <t>E. stage triumphs of an astonishing player</t>
+  </si>
+  <si>
+    <t>A. the stage personalities of the past would appeal on  a personal level to people like the author</t>
+  </si>
+  <si>
+    <t>B. their contemporaries would have understood famous actors</t>
+  </si>
+  <si>
+    <t>C. the acting of famous stage personalities would appeal to us today </t>
+  </si>
+  <si>
+    <t>D. Garrick was as great as he is portrayed </t>
+  </si>
+  <si>
+    <t>E. historical records can reveal personality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. I only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. II only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C. I and III only </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.  II and III only </t>
+  </si>
+  <si>
+    <t>E.  I, II and III</t>
+  </si>
+  <si>
+    <t>A. 90</t>
+  </si>
+  <si>
+    <t>B. 95</t>
+  </si>
+  <si>
+    <t>C. 100</t>
+  </si>
+  <si>
+    <t>D. 105</t>
+  </si>
+  <si>
+    <t>E. 110</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -808,15 +604,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="SimSun"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -857,15 +654,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -875,15 +672,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,14 +693,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1212,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1251,18 +1052,18 @@
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="7" t="s">
@@ -1275,12 +1076,14 @@
         <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1289,12 +1092,14 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I3" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1303,12 +1108,14 @@
         <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1317,12 +1124,14 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I5" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
@@ -1331,359 +1140,429 @@
         <v>17</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="7" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="10" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>3</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="15"/>
+        <v>79</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="D12" s="16" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>37</v>
+        <v>93</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>11</v>
+      <c r="B17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="G17" s="14"/>
       <c r="H17" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D18" s="7" t="s">
-        <v>40</v>
+        <v>83</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="D19" s="7" t="s">
-        <v>41</v>
+        <v>83</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>45</v>
+        <v>83</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="D21" s="10" t="s">
-        <v>43</v>
+        <v>83</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="12" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>5</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" s="15"/>
+        <v>79</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="D22" s="16" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
-        <v>49</v>
+        <v>83</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D24" s="7" t="s">
-        <v>50</v>
+        <v>83</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D26" s="10" t="s">
-        <v>52</v>
+        <v>83</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="12" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>6</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>116</v>
+      <c r="B27" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="10" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="D30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="D31" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>109</v>
+        <v>82</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1691,271 +1570,538 @@
         <v>7</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="D36" s="10" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="12" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>8</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="D41" s="10" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="12" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>9</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="D46" s="10" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="E46" s="13"/>
       <c r="F46" s="13" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="4:8" ht="40.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" ht="40.5" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="4:8" ht="40.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" ht="40.5" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I106" s="4"/>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I112" s="4"/>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I113" s="4"/>
+    </row>
+    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I115" s="4"/>
+    </row>
+    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I119" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A6"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H51">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6 H12:H26 H32:H51">
       <formula1>"SC,CR,RC,Quant"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11 H27:H31">
+      <formula1>"SC,CR,RC,Q"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add sample question sub-type for questions
</commit_message>
<xml_diff>
--- a/SC 1 - 10 - Commented.xlsx
+++ b/SC 1 - 10 - Commented.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="105">
   <si>
     <t>Stimulus</t>
   </si>
@@ -250,21 +250,6 @@
     <t>E. creatures of the seabed that were suffering because food supplies were dwindling, which possibly resulted from increasing</t>
   </si>
   <si>
-    <t xml:space="preserve">A. the brain growing in mice when placed in a stimulating environment or neurons increasing in canaries that </t>
-  </si>
-  <si>
-    <t>B. mice whose brains grow when they are placed in a stimulating environment or canaries whose neurons increase when they</t>
-  </si>
-  <si>
-    <t>C. mice's brains that grow when they are placed in a stimulating environment or canaries' neurons that increase when they</t>
-  </si>
-  <si>
-    <t>D. the brain growth in mice when placed in a stimulating environment or the increase in canaries' neurons when they</t>
-  </si>
-  <si>
-    <t>E. brain growth in mice that are placed in a stimulating environment or an increase in neurons in canaries that</t>
-  </si>
-  <si>
     <t>D. Nghĩa của câu hướng tới việc nghiên cứu hé lộ việc các loài sinh vật đang chịu đựng vì nguồn cung thức ăn suy giảm, không phải nghiên cứu hé lộ về loài sinh vật có tính chất như thế, vì vậy câu phải có "that".</t>
   </si>
   <si>
@@ -275,21 +260,6 @@
   </si>
   <si>
     <t>A. Việc các sinh vật phải chịu đựng từ nguồn thức ăn giảm là không hợp lý, cần phải là nguồn thức ăn giảm là nguyên nhân gây ra điều gì đó, rồi tiếp tục làm các sinh vật phải chịu đựng.</t>
-  </si>
-  <si>
-    <t>B. neurogenesis không thể bao gồm "mice" và "canaries", mà phải là "brain growth" và "an increase in neurons"</t>
-  </si>
-  <si>
-    <t>C. 2 từ "they" trong đáp án này chỉ tới 2 đối tượng khác nhau (mice vầ canaries). Bên cạnh đó, pronoun "they" không thể chỉ tới một đối tượng nằm trong dấu sở hữu cách</t>
-  </si>
-  <si>
-    <t>D. Từ "they" không thể chỉ tới một đối tượng nằm trong dấu sở hữu cách (canaries's)</t>
-  </si>
-  <si>
-    <t>A. Đối tượng so sánh trong câu là sự tăng trưởng trong não và sự tăng lên trong neurons, đối tượng so sánh không phải là não và neurons.</t>
-  </si>
-  <si>
-    <t>E. Đáp án đúng. So sánh "brain growth" với "an increase in neurons" là hoàn toàn hợp lý</t>
   </si>
   <si>
     <t>Type</t>
@@ -408,32 +378,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Recently documented examples of neurogenesis, the production of new brain cells, include</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the brain growing in mice when placed in a stimulating environment or neurons increasing in canaries that</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> learn new songs.</t>
-    </r>
-  </si>
-  <si>
     <t>If an object travels at five feet per second, how many feet does it travel in one hour?</t>
   </si>
   <si>
@@ -568,6 +512,21 @@
   </si>
   <si>
     <t>MISC</t>
+  </si>
+  <si>
+    <t>ARTH</t>
+  </si>
+  <si>
+    <t>INF</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A poultry farm has only chickens and pigs. When the manager of the poultry counted the heads of the stock in the farm, the number totalled up to 200. However, when the number of legs was counted, the number totalled up to 540. How many more chickens were there in the farm? Note: Each pig had 4 legs and each chicken had 2 legs.</t>
+  </si>
+  <si>
+    <t>ALG</t>
   </si>
 </sst>
 </file>
@@ -1015,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +986,7 @@
     <col min="5" max="5" width="14.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="50" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="4" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -1037,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1052,10 +1011,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1063,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="7" t="s">
@@ -1076,10 +1035,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1092,10 +1051,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1108,10 +1067,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1124,10 +1083,10 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1140,10 +1099,10 @@
         <v>17</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1151,83 +1110,83 @@
         <v>2</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="10" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="12" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -1235,67 +1194,67 @@
         <v>3</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>90</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,18 +1262,18 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="12" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1322,83 +1281,83 @@
         <v>4</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>95</v>
-      </c>
       <c r="E17" s="15" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="19" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="19" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="20" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="12" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -1406,82 +1365,82 @@
         <v>5</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="19" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="19" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="19" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="12" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1489,80 +1448,80 @@
         <v>6</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="10" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="12" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1570,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
@@ -1583,10 +1542,10 @@
         <v>24</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
@@ -1597,10 +1556,10 @@
         <v>25</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1611,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1625,10 +1584,10 @@
         <v>26</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1640,10 +1599,10 @@
         <v>27</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1651,7 +1610,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
@@ -1664,10 +1623,10 @@
         <v>33</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
@@ -1678,10 +1637,10 @@
         <v>35</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1692,10 +1651,10 @@
         <v>36</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1706,10 +1665,10 @@
         <v>38</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1721,10 +1680,10 @@
         <v>37</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1732,7 +1691,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
@@ -1742,13 +1701,13 @@
         <v>10</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
@@ -1759,10 +1718,10 @@
         <v>18</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1770,13 +1729,13 @@
         <v>41</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1784,13 +1743,13 @@
         <v>42</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1799,93 +1758,93 @@
       </c>
       <c r="E46" s="13"/>
       <c r="F46" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>60</v>
-      </c>
       <c r="I46" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="1">
+        <v>70</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="1">
+        <v>120</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <v>60</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D50" s="1">
+        <v>130</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="4:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="4:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H50" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="4:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D51" s="1">
+        <v>80</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.25">
@@ -2097,10 +2056,10 @@
     <mergeCell ref="A2:A6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6 H12:H26 H32:H51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6 H12:H26 H32:H46">
       <formula1>"SC,CR,RC,Quant"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11 H27:H31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11 H27:H31 H47:H51">
       <formula1>"SC,CR,RC,Q"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>